<commit_message>
Update bahasa + table
</commit_message>
<xml_diff>
--- a/public/RPKC.xlsx
+++ b/public/RPKC.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -41,13 +41,16 @@
     <t>HCO</t>
   </si>
   <si>
+    <t>berubah pelatihan</t>
+  </si>
+  <si>
+    <t>ARI GUNAWAN GUNAIDI</t>
+  </si>
+  <si>
+    <t>HRD</t>
+  </si>
+  <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>ARI GUNAWAN GUNAIDI</t>
-  </si>
-  <si>
-    <t>HRD</t>
   </si>
   <si>
     <t>UI/UX Design Training</t>
@@ -472,7 +475,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -483,13 +486,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -500,13 +503,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -517,13 +520,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -531,16 +534,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -551,13 +554,13 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -565,16 +568,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -582,7 +585,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -591,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -599,7 +602,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -608,7 +611,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -616,7 +619,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -625,7 +628,7 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -633,16 +636,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -650,16 +653,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -667,16 +670,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>